<commit_message>
updating deliveries for 3d modeling
</commit_message>
<xml_diff>
--- a/MCET0220/exam_3.xlsx
+++ b/MCET0220/exam_3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="178">
   <si>
     <r>
       <rPr>
@@ -231,6 +231,9 @@
     <t xml:space="preserve">Part b)    Determine the smallest force P required to start the block moving if the Cable AB is removed</t>
   </si>
   <si>
+    <t xml:space="preserve">Assume:</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -326,6 +329,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Ridig bodies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ideal pins</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -451,10 +460,16 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Assume</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ideal joint and ideal cord</t>
   </si>
   <si>
     <t xml:space="preserve">Rigid rod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D rod</t>
   </si>
   <si>
     <t xml:space="preserve">List coordinates</t>
@@ -696,6 +711,27 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">hT =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bT =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l2 =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2 =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l3 =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3 =</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -864,6 +900,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">dCD =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dCF =</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using the method of sections, determine the force in members BC, CF and FG</t>
   </si>
   <si>
@@ -900,6 +942,39 @@
     <t xml:space="preserve">Record results in table below</t>
   </si>
   <si>
+    <t xml:space="preserve">Ridid bodies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weightless truss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideal pins and roller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equations to the right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGFx =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGF =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FGFy =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCFy =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCF =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCFx =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCB =</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tension or 
 Compression</t>
   </si>
@@ -907,10 +982,19 @@
     <t xml:space="preserve">FBC</t>
   </si>
   <si>
+    <t xml:space="preserve">Tension</t>
+  </si>
+  <si>
     <t xml:space="preserve">FCF</t>
   </si>
   <si>
+    <t xml:space="preserve">Tesnion</t>
+  </si>
+  <si>
     <t xml:space="preserve">FFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compression</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2225,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>112320</xdr:rowOff>
     </xdr:from>
@@ -2162,8 +2246,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2576520" y="112320"/>
-          <a:ext cx="4519440" cy="3296160"/>
+          <a:off x="2576880" y="112320"/>
+          <a:ext cx="4519080" cy="3296160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>365040</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>65160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11880</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>127440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Image 14" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5147640" y="3531960"/>
+          <a:ext cx="2955960" cy="1766880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2185,17 +2306,17 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>476280</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>75600</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 3" descr=""/>
+        <xdr:cNvPr id="19" name="Picture 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2204,8 +2325,156 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="808920" y="336240"/>
+          <a:off x="808920" y="336600"/>
           <a:ext cx="6675120" cy="3287880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>316440</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>17280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Image 15" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="332640" y="8070840"/>
+          <a:ext cx="3723120" cy="2228040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>118440</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>174240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>482400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>135720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Image 16" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8138160" y="7757280"/>
+          <a:ext cx="4644720" cy="1136160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>236880</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>125640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>108000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Image 17" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8256600" y="9067680"/>
+          <a:ext cx="4151880" cy="1170720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266760</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>174240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>82800</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>208800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Image 18" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8286480" y="10455840"/>
+          <a:ext cx="3485160" cy="2818440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2237,7 +2506,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="image3.jpg" descr=""/>
+        <xdr:cNvPr id="24" name="image3.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2275,7 +2544,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="image2.jpg" descr=""/>
+        <xdr:cNvPr id="25" name="image2.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2313,7 +2582,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="image4.jpg" descr=""/>
+        <xdr:cNvPr id="26" name="image4.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2351,7 +2620,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="image1.jpg" descr=""/>
+        <xdr:cNvPr id="27" name="image1.jpg" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2394,7 +2663,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 28" descr=""/>
+        <xdr:cNvPr id="28" name="Picture 28" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2431,7 +2700,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 30" descr=""/>
+        <xdr:cNvPr id="29" name="Picture 30" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2463,7 +2732,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2490,8 +2759,8 @@
   </sheetPr>
   <dimension ref="C1:Z93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G89" activeCellId="0" sqref="G89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K65" activeCellId="0" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3700,7 +3969,9 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
+      <c r="K65" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="L65" s="5"/>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
@@ -3969,7 +4240,7 @@
     </row>
     <row r="82" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="14"/>
@@ -4004,7 +4275,7 @@
     <row r="84" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E84" s="5" t="n">
         <f aca="false">D24</f>
@@ -4216,8 +4487,8 @@
   </sheetPr>
   <dimension ref="C1:V62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4232,7 +4503,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -4480,7 +4751,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="7" t="n">
         <v>200</v>
@@ -4498,7 +4769,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="7" t="n">
         <f aca="false">DEGREES(ATAN(0.8/1.7))</f>
@@ -4659,7 +4930,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="2"/>
@@ -4673,7 +4944,7 @@
     </row>
     <row r="33" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="2"/>
@@ -4701,7 +4972,9 @@
       <c r="C35" s="13"/>
       <c r="D35" s="29"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -4713,7 +4986,9 @@
       <c r="C36" s="13"/>
       <c r="D36" s="29"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -4725,7 +5000,9 @@
       <c r="C37" s="13"/>
       <c r="D37" s="29"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -4737,7 +5014,9 @@
       <c r="C38" s="13"/>
       <c r="D38" s="29"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -4807,7 +5086,7 @@
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -4937,7 +5216,7 @@
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="19" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D54" s="19" t="n">
         <f aca="false">D19</f>
@@ -4956,13 +5235,13 @@
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="19" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D55" s="19" t="n">
         <v>1</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="30"/>
@@ -4974,7 +5253,7 @@
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="19" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D56" s="19" t="n">
         <f aca="false">2*D19/(1.7*SIN(RADIANS(D20)))</f>
@@ -4984,7 +5263,7 @@
         <v>17</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G56" s="30"/>
       <c r="H56" s="30"/>
@@ -4995,7 +5274,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D57" s="19" t="n">
         <f aca="false">D20</f>
@@ -5014,7 +5293,7 @@
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D58" s="19" t="n">
         <f aca="false">-D56*COS(RADIANS(D57))</f>
@@ -5024,7 +5303,7 @@
         <v>17</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G58" s="30"/>
       <c r="H58" s="30"/>
@@ -5035,7 +5314,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D59" s="19" t="n">
         <f aca="false">D19 - D56*SIN(RADIANS(D57))</f>
@@ -5045,7 +5324,7 @@
         <v>17</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G59" s="30"/>
       <c r="H59" s="30"/>
@@ -5056,7 +5335,7 @@
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D60" s="19" t="n">
         <f aca="false">SQRT(D58^2 + D59^2)</f>
@@ -5075,7 +5354,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D61" s="19" t="n">
         <f aca="false">DEGREES(ATAN(D59/D58))</f>
@@ -5085,7 +5364,7 @@
         <v>14</v>
       </c>
       <c r="F61" s="32" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G61" s="30"/>
       <c r="H61" s="30"/>
@@ -5125,8 +5404,8 @@
   </sheetPr>
   <dimension ref="C1:V115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L99" activeCellId="0" sqref="L99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5140,7 +5419,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -5356,7 +5635,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -5388,7 +5667,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D19" s="7" t="n">
         <v>500</v>
@@ -5444,7 +5723,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -5463,7 +5742,9 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -5476,7 +5757,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -5490,7 +5771,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -5503,7 +5784,9 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -5630,7 +5913,7 @@
     </row>
     <row r="38" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="33" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="2"/>
@@ -5645,13 +5928,13 @@
     <row r="39" s="34" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="35"/>
       <c r="D39" s="35" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G39" s="36"/>
       <c r="H39" s="36"/>
@@ -5662,7 +5945,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="19" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D40" s="19" t="n">
         <v>0</v>
@@ -5682,7 +5965,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="19" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D41" s="19" t="n">
         <v>0</v>
@@ -5702,7 +5985,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="19" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D42" s="19" t="n">
         <v>0</v>
@@ -5722,7 +6005,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="19" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D43" s="19" t="n">
         <v>2</v>
@@ -5742,7 +6025,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D44" s="19" t="n">
         <v>2</v>
@@ -5762,7 +6045,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="19" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D45" s="19" t="n">
         <v>-4</v>
@@ -5782,7 +6065,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="19" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D46" s="19" t="n">
         <v>0</v>
@@ -5814,7 +6097,7 @@
     </row>
     <row r="48" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="2"/>
@@ -5828,7 +6111,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30"/>
@@ -5842,7 +6125,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30"/>
@@ -5872,7 +6155,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="37" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30"/>
@@ -5899,17 +6182,17 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="35"/>
       <c r="D54" s="35" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E54" s="35" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F54" s="35" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G54" s="30"/>
       <c r="H54" s="30" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I54" s="30" t="n">
         <f aca="false">SQRT(D58^2 + E58^2 + F58^2)</f>
@@ -5921,7 +6204,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="19" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D55" s="19" t="n">
         <f aca="false">D42-D40</f>
@@ -5937,7 +6220,7 @@
       </c>
       <c r="G55" s="30"/>
       <c r="H55" s="30" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="I55" s="30" t="n">
         <f aca="false">SQRT(D59^2 + E59^2 + F59^2)</f>
@@ -5949,7 +6232,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="19" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D56" s="19" t="n">
         <f aca="false">D46-D40</f>
@@ -5965,7 +6248,7 @@
       </c>
       <c r="G56" s="30"/>
       <c r="H56" s="30" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I56" s="30" t="n">
         <f aca="false">SQRT(D60^2 + E60^2 + F60^2)</f>
@@ -5977,7 +6260,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="19" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D57" s="19" t="n">
         <f aca="false">D41-D40</f>
@@ -6000,7 +6283,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="19" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D58" s="19" t="n">
         <f aca="false">D45-D42</f>
@@ -6023,7 +6306,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="19" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D59" s="19" t="n">
         <f aca="false">D43-D46</f>
@@ -6046,7 +6329,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="19" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D60" s="19" t="n">
         <f aca="false">D44-D41</f>
@@ -6069,7 +6352,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="19" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D61" s="19" t="n">
         <f aca="false">D58/I54</f>
@@ -6092,7 +6375,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="19" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D62" s="19" t="n">
         <f aca="false">D59/I55</f>
@@ -6115,7 +6398,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="19" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D63" s="19" t="n">
         <f aca="false">D60/I56</f>
@@ -6152,32 +6435,32 @@
       <c r="C65" s="39"/>
       <c r="D65" s="39"/>
       <c r="E65" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H65" s="39"/>
       <c r="I65" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J65" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K65" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="L65" s="39"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="16" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E66" s="19" t="n">
         <f aca="false">D56</f>
@@ -6192,7 +6475,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I66" s="19" t="n">
         <f aca="false">F66*G67 - F67* G66</f>
@@ -6245,32 +6528,32 @@
       <c r="C69" s="39"/>
       <c r="D69" s="39"/>
       <c r="E69" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H69" s="39"/>
       <c r="I69" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J69" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K69" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="L69" s="30"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="16" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E70" s="19" t="n">
         <f aca="false">D55</f>
@@ -6285,7 +6568,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I70" s="19" t="n">
         <f aca="false">F70*G71 - F71* G70</f>
@@ -6338,32 +6621,32 @@
       <c r="C73" s="39"/>
       <c r="D73" s="39"/>
       <c r="E73" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H73" s="39"/>
       <c r="I73" s="19" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="L73" s="30"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="16" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E74" s="19" t="n">
         <f aca="false">D57</f>
@@ -6378,7 +6661,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="30" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I74" s="19" t="n">
         <f aca="false">F74*G75 - F75* G74</f>
@@ -6501,7 +6784,7 @@
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30"/>
@@ -6515,7 +6798,7 @@
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -6529,7 +6812,7 @@
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="30" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D85" s="26"/>
       <c r="E85" s="44"/>
@@ -6543,7 +6826,7 @@
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="30" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D86" s="26"/>
       <c r="E86" s="44"/>
@@ -6698,15 +6981,15 @@
       <c r="J98" s="30"/>
       <c r="K98" s="30"/>
       <c r="L98" s="30" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="M98" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="37" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D99" s="26"/>
       <c r="E99" s="44"/>
@@ -6721,33 +7004,33 @@
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="39"/>
       <c r="D100" s="39" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E100" s="26" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F100" s="39" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G100" s="39" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H100" s="39" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="I100" s="39" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="J100" s="30"/>
       <c r="K100" s="30"/>
       <c r="L100" s="30"/>
       <c r="M100" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="39" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D101" s="45" t="n">
         <v>1</v>
@@ -6774,12 +7057,12 @@
       <c r="K101" s="30"/>
       <c r="L101" s="30"/>
       <c r="M101" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="39" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D102" s="49" t="n">
         <v>0</v>
@@ -6806,12 +7089,12 @@
       <c r="K102" s="30"/>
       <c r="L102" s="30"/>
       <c r="M102" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="39" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D103" s="49" t="n">
         <v>0</v>
@@ -6838,12 +7121,12 @@
       <c r="K103" s="30"/>
       <c r="L103" s="30"/>
       <c r="M103" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="39" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D104" s="49" t="n">
         <v>0</v>
@@ -6870,12 +7153,12 @@
       <c r="K104" s="30"/>
       <c r="L104" s="30"/>
       <c r="M104" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="39" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D105" s="49" t="n">
         <v>0</v>
@@ -6901,12 +7184,12 @@
       <c r="K105" s="30"/>
       <c r="L105" s="30"/>
       <c r="M105" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="39" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D106" s="51" t="n">
         <v>0</v>
@@ -6965,7 +7248,7 @@
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="19" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D109" s="21" t="n">
         <v>646.5</v>
@@ -6983,7 +7266,7 @@
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="19" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D110" s="21" t="n">
         <v>433.3</v>
@@ -7001,7 +7284,7 @@
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C111" s="19" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D111" s="35" t="n">
         <v>218.7</v>
@@ -7019,7 +7302,7 @@
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D112" s="21" t="n">
         <v>1327.3</v>
@@ -7037,7 +7320,7 @@
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="19" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D113" s="21" t="n">
         <v>-58.5</v>
@@ -7055,7 +7338,7 @@
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="19" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D114" s="23" t="n">
         <f aca="false">SQRT(D111^2+D112^2 +D113^2)</f>
@@ -7103,8 +7386,8 @@
   </sheetPr>
   <dimension ref="C1:U67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7117,7 +7400,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -7313,9 +7596,15 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -7323,10 +7612,16 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+    <row r="17" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -7334,10 +7629,16 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+    <row r="18" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -7345,10 +7646,16 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+    <row r="19" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -7356,10 +7663,16 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+    <row r="20" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -7368,9 +7681,15 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>55</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -7404,7 +7723,7 @@
     </row>
     <row r="24" s="4" customFormat="true" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="12" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="11"/>
@@ -7439,69 +7758,129 @@
     </row>
     <row r="27" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="54" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D27" s="54" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="E27" s="54" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
+    <row r="28" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="55" t="n">
+        <f aca="false">D16*D17/2</f>
+        <v>2475</v>
+      </c>
+      <c r="E28" s="55" t="n">
+        <f aca="false">D16/3</f>
+        <v>36.6666666666667</v>
+      </c>
+      <c r="F28" s="55" t="n">
+        <f aca="false">40 +D17/3</f>
+        <v>55</v>
+      </c>
+      <c r="G28" s="55" t="n">
+        <f aca="false">D28*E28</f>
+        <v>90750</v>
+      </c>
+      <c r="H28" s="55" t="n">
+        <f aca="false">D28*F28</f>
+        <v>136125</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
+    <row r="29" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="54" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="55" t="n">
+        <f aca="false">D18*D19</f>
+        <v>1100</v>
+      </c>
+      <c r="E29" s="55" t="n">
+        <f aca="false">D19/2</f>
+        <v>55</v>
+      </c>
+      <c r="F29" s="55" t="n">
+        <f aca="false">D20+D18/2</f>
+        <v>35</v>
+      </c>
+      <c r="G29" s="55" t="n">
+        <f aca="false">D29*E29</f>
+        <v>60500</v>
+      </c>
+      <c r="H29" s="55" t="n">
+        <f aca="false">D29*F29</f>
+        <v>38500</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
+    <row r="30" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="54" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" s="55" t="n">
+        <f aca="false">D20*D21</f>
+        <v>1650</v>
+      </c>
+      <c r="E30" s="55" t="n">
+        <f aca="false">55 + D21/2</f>
+        <v>82.5</v>
+      </c>
+      <c r="F30" s="55" t="n">
+        <f aca="false">D20/2</f>
+        <v>15</v>
+      </c>
+      <c r="G30" s="55" t="n">
+        <f aca="false">D30*E30</f>
+        <v>136125</v>
+      </c>
+      <c r="H30" s="55" t="n">
+        <f aca="false">D30*F30</f>
+        <v>24750</v>
+      </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
     <row r="31" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" s="55"/>
+        <v>139</v>
+      </c>
+      <c r="D31" s="55" t="n">
+        <f aca="false">D28+D29+D30</f>
+        <v>5225</v>
+      </c>
       <c r="E31" s="55"/>
       <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
+      <c r="G31" s="55" t="n">
+        <f aca="false">G28+G29+G30</f>
+        <v>287375</v>
+      </c>
+      <c r="H31" s="55" t="n">
+        <f aca="false">H28+H29+H30</f>
+        <v>199375</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -7519,7 +7898,7 @@
     </row>
     <row r="33" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="56" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -7549,10 +7928,15 @@
     </row>
     <row r="35" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
+        <v>141</v>
+      </c>
+      <c r="D35" s="19" t="n">
+        <f aca="false">G31/D31</f>
+        <v>55</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>126</v>
+      </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -7562,10 +7946,15 @@
     </row>
     <row r="36" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+        <v>142</v>
+      </c>
+      <c r="D36" s="19" t="n">
+        <f aca="false">H31/D31</f>
+        <v>38.1578947368421</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>126</v>
+      </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
@@ -7586,7 +7975,7 @@
     </row>
     <row r="38" s="4" customFormat="true" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="12" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="11"/>
@@ -7610,71 +7999,149 @@
     </row>
     <row r="40" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="54" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E40" s="58" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="F40" s="54" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="G40" s="54" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="H40" s="54" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="J40" s="54" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="54"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
+    <row r="41" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="55" t="n">
+        <f aca="false">1/12*D16*D17^3</f>
+        <v>835312.5</v>
+      </c>
+      <c r="E41" s="55" t="n">
+        <f aca="false">1/12*D17*D16^3</f>
+        <v>4991250</v>
+      </c>
+      <c r="F41" s="55" t="n">
+        <f aca="false">D28</f>
+        <v>2475</v>
+      </c>
+      <c r="G41" s="55" t="n">
+        <f aca="false">E28-D35</f>
+        <v>-18.3333333333333</v>
+      </c>
+      <c r="H41" s="55" t="n">
+        <f aca="false">F28-D36</f>
+        <v>16.8421052631579</v>
+      </c>
+      <c r="I41" s="55" t="n">
+        <f aca="false">F41*G41^2</f>
+        <v>831875</v>
+      </c>
+      <c r="J41" s="55" t="n">
+        <f aca="false">F41*H41^2</f>
+        <v>702049.861495845</v>
+      </c>
       <c r="K41" s="59"/>
     </row>
-    <row r="42" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="54"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
+    <row r="42" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="54" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" s="55" t="n">
+        <f aca="false">1/3*D19*D18^3</f>
+        <v>36666.6666666667</v>
+      </c>
+      <c r="E42" s="55" t="n">
+        <f aca="false">1/3*D18*D19^3</f>
+        <v>4436666.66666667</v>
+      </c>
+      <c r="F42" s="55" t="n">
+        <f aca="false">D29</f>
+        <v>1100</v>
+      </c>
+      <c r="G42" s="55" t="n">
+        <f aca="false">E29-D35</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="55" t="n">
+        <f aca="false">F29-D36</f>
+        <v>-3.1578947368421</v>
+      </c>
+      <c r="I42" s="55" t="n">
+        <f aca="false">F42*G42^2</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="55" t="n">
+        <f aca="false">F42*H42^2</f>
+        <v>10969.5290858726</v>
+      </c>
       <c r="K42" s="59"/>
     </row>
-    <row r="43" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="54"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="55"/>
+    <row r="43" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="54" t="n">
+        <v>3</v>
+      </c>
+      <c r="D43" s="55" t="n">
+        <f aca="false">1/3*D21*D20^3</f>
+        <v>495000</v>
+      </c>
+      <c r="E43" s="55" t="n">
+        <f aca="false">1/3*D20*D21^3</f>
+        <v>1663750</v>
+      </c>
+      <c r="F43" s="55" t="n">
+        <f aca="false">D30</f>
+        <v>1650</v>
+      </c>
+      <c r="G43" s="55" t="n">
+        <f aca="false">E30-D35</f>
+        <v>27.5</v>
+      </c>
+      <c r="H43" s="55" t="n">
+        <f aca="false">F30-D36</f>
+        <v>-23.1578947368421</v>
+      </c>
+      <c r="I43" s="55" t="n">
+        <f aca="false">F43*G43^2</f>
+        <v>1247812.5</v>
+      </c>
+      <c r="J43" s="55" t="n">
+        <f aca="false">F43*H43^2</f>
+        <v>884875.346260388</v>
+      </c>
       <c r="K43" s="59"/>
     </row>
     <row r="44" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
+        <v>139</v>
+      </c>
+      <c r="D44" s="55" t="n">
+        <f aca="false">D41+D42+D43</f>
+        <v>1366979.16666667</v>
+      </c>
+      <c r="E44" s="55" t="n">
+        <f aca="false">E41+E42+E43</f>
+        <v>11091666.6666667</v>
+      </c>
+      <c r="F44" s="55" t="n">
+        <f aca="false">F41+F42+F43</f>
+        <v>5225</v>
+      </c>
       <c r="G44" s="55"/>
       <c r="H44" s="55"/>
       <c r="I44" s="55"/>
@@ -7694,7 +8161,7 @@
     </row>
     <row r="46" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="56" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -7724,7 +8191,7 @@
     </row>
     <row r="48" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="60" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
@@ -7737,7 +8204,7 @@
     </row>
     <row r="49" s="4" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="60" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
@@ -7965,8 +8432,8 @@
   </sheetPr>
   <dimension ref="C1:W68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F68" activeCellId="0" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7981,7 +8448,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -8219,12 +8686,12 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="2"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -8232,12 +8699,18 @@
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="2"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -8246,9 +8719,15 @@
       <c r="M18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="62"/>
+      <c r="C19" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>52</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -8392,7 +8871,7 @@
     </row>
     <row r="30" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="12" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="2"/>
@@ -8407,7 +8886,7 @@
     </row>
     <row r="31" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="56" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="2"/>
@@ -8422,7 +8901,7 @@
     </row>
     <row r="32" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="63" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="2"/>
@@ -8437,7 +8916,7 @@
     </row>
     <row r="33" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="15" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="2"/>
@@ -8452,7 +8931,7 @@
     </row>
     <row r="34" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="64" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="2"/>
@@ -8498,7 +8977,9 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -8511,7 +8992,9 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -8524,7 +9007,9 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="I39" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -8537,7 +9022,9 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -8622,7 +9109,9 @@
       <c r="M46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>163</v>
+      </c>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
@@ -8648,8 +9137,13 @@
       <c r="M48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="C49" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" s="16" t="n">
+        <f aca="false">2000*D18/D19</f>
+        <v>4000</v>
+      </c>
       <c r="E49" s="16"/>
       <c r="F49" s="16"/>
       <c r="G49" s="30"/>
@@ -8661,8 +9155,13 @@
       <c r="M49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="24"/>
-      <c r="D50" s="25"/>
+      <c r="C50" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" s="25" t="n">
+        <f aca="false">D49*SQRT(5)</f>
+        <v>8944.27190999916</v>
+      </c>
       <c r="E50" s="26"/>
       <c r="F50" s="22"/>
       <c r="G50" s="30"/>
@@ -8673,9 +9172,14 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="12"/>
-      <c r="D51" s="29"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <f aca="false">D50/SQRT(2)</f>
+        <v>6324.55532033676</v>
+      </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -8686,9 +9190,14 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="12"/>
-      <c r="D52" s="29"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" s="16" t="n">
+        <f aca="false">-4000 + D51</f>
+        <v>2324.55532033676</v>
+      </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -8699,9 +9208,14 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="13"/>
-      <c r="D53" s="29"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="16" t="n">
+        <f aca="false">D52*SQRT(2)</f>
+        <v>3287.41766050678</v>
+      </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -8712,9 +9226,14 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="13"/>
-      <c r="D54" s="29"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D54" s="16" t="n">
+        <f aca="false">D53/SQRT(2)</f>
+        <v>2324.55532033676</v>
+      </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -8725,9 +9244,14 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="13"/>
-      <c r="D55" s="29"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="16" t="n">
+        <f aca="false">D49-D54</f>
+        <v>1675.44467966324</v>
+      </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -8738,9 +9262,9 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="13"/>
-      <c r="D56" s="29"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -8751,9 +9275,9 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="13"/>
-      <c r="D57" s="29"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -8764,9 +9288,9 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="13"/>
-      <c r="D58" s="29"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -8777,9 +9301,9 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="13"/>
-      <c r="D59" s="29"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -8853,7 +9377,7 @@
         <v>6</v>
       </c>
       <c r="F64" s="66" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -8865,11 +9389,18 @@
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
+        <v>172</v>
+      </c>
+      <c r="D65" s="19" t="n">
+        <f aca="false">D55</f>
+        <v>1675.44467966324</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -8880,11 +9411,18 @@
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
+        <v>174</v>
+      </c>
+      <c r="D66" s="19" t="n">
+        <f aca="false">D53</f>
+        <v>3287.41766050678</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>175</v>
+      </c>
       <c r="G66" s="30"/>
       <c r="H66" s="30"/>
       <c r="I66" s="30"/>
@@ -8895,11 +9433,18 @@
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="D67" s="19" t="n">
+        <f aca="false">D50</f>
+        <v>8944.27190999916</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
       <c r="I67" s="30"/>
@@ -8940,7 +9485,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="W16" activeCellId="0" sqref="W16"/>
     </sheetView>
   </sheetViews>
@@ -8967,7 +9512,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AA22" activeCellId="0" sqref="AA22"/>
     </sheetView>
   </sheetViews>

</xml_diff>